<commit_message>
Vector_Comp.py - Fixed error in calculation of scale factor (2d & 3d vector magnitude calculation indices were wrong)
</commit_message>
<xml_diff>
--- a/Points_2d.csv.xlsx
+++ b/Points_2d.csv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\Current\PPM_TM\PPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scpt1\PPM_TM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CFCF27-634A-4D3B-B5F4-8735C37AD407}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5EA8E-F20A-4FD0-B90F-8AA352298D82}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6618" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -973,12 +973,20 @@
       <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.25</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>

</xml_diff>

<commit_message>
Vector_Comp.py - small fix to bring s1 & s2 into alignment w/ scale; print statement & comment clean-up
</commit_message>
<xml_diff>
--- a/Points_2d.csv.xlsx
+++ b/Points_2d.csv.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scpt1\PPM_TM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D5EA8E-F20A-4FD0-B90F-8AA352298D82}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89941DBD-8CD0-4BC8-BEBD-B8ED48B4B7EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6618" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Points_2d" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -886,7 +886,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -974,10 +974,12 @@
         <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>3.5</v>
+        <f>3.75-0.0701941</f>
+        <v>3.6798058999999999</v>
       </c>
       <c r="D8" s="2">
-        <v>3.5</v>
+        <f>3.5 - 0.0548058971</f>
+        <v>3.4451941028999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -985,7 +987,7 @@
         <v>1.25</v>
       </c>
       <c r="B9" s="2">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>

</xml_diff>